<commit_message>
difúzní přezkum: + table
</commit_message>
<xml_diff>
--- a/data/publikace.xlsx
+++ b/data/publikace.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarom\Documents\GitHub\jfronc.cz\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64D17FB-07AA-4FC5-A7D4-D6A6DF8F09D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6966FE-0408-4735-9530-D1EEA0BB5313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A6FCB930-9EF3-4AF5-902E-F9B54FCB8C2A}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A6FCB930-9EF3-4AF5-902E-F9B54FCB8C2A}"/>
   </bookViews>
   <sheets>
     <sheet name="publikace" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="82">
   <si>
     <t>Item Type</t>
   </si>
@@ -133,9 +133,6 @@
     <t>Praha</t>
   </si>
   <si>
-    <t>Žák Krzyžanková, Katarzyna a kol.</t>
-  </si>
-  <si>
     <t>Hledání smysluplné zákonné úpravy přezkumu krizových opatření a nouzového stavu</t>
   </si>
   <si>
@@ -215,6 +212,60 @@
   </si>
   <si>
     <t>https://www.ilaw.cas.cz/upload/web/files/pravnik/issues/2024/6/3_Fronc_587-604_6_2024.pdf</t>
+  </si>
+  <si>
+    <t>Partnerství pro všechny: K diskriminační povaze výlučně stejnopohlavních svazků</t>
+  </si>
+  <si>
+    <t>Kulturní války z pohledu ústavního práva</t>
+  </si>
+  <si>
+    <t>Žák Krzyžanková, Katarzyna a kol</t>
+  </si>
+  <si>
+    <t>Volební geometrie v Předlitavsku</t>
+  </si>
+  <si>
+    <t>Fabini, Pavel, Zouzal, Tomáš (eds)</t>
+  </si>
+  <si>
+    <t>Vše pro mandát? Podvody, korupce a násilí při parlamentních volbách ve střední Evropě v 19. a 20. století</t>
+  </si>
+  <si>
+    <t>Masarykův ústav a Archiv AV ČR</t>
+  </si>
+  <si>
+    <t>Ústavní konformita nového stavebního zákona</t>
+  </si>
+  <si>
+    <t>Referendum v dějinách Spojeného království</t>
+  </si>
+  <si>
+    <t>Ústavní mantinely pro státní politiku</t>
+  </si>
+  <si>
+    <t>Brexit v zrcadle ústavního práva</t>
+  </si>
+  <si>
+    <t>Kdy je proporcionální bránit sebepoškozování?</t>
+  </si>
+  <si>
+    <t>Kdy se senátor musí stát poslancem?</t>
+  </si>
+  <si>
+    <t>Poměřování základních práv</t>
+  </si>
+  <si>
+    <t>Problémy parlamentarismu</t>
+  </si>
+  <si>
+    <t>Univerzita Karlova, Právnická fakulta</t>
+  </si>
+  <si>
+    <t>https://www.jurisprudence.cz/cz/casopis/difuzni-prezkum-okrajova-nesouladnost-a-pravni-jistota.m-565.html</t>
+  </si>
+  <si>
+    <t>https://www.jurisprudence.cz/cz/casopis/difuzni-prezkum-okrajova-nesouladnost-a-pravni-jistota.dm-565.pdf</t>
   </si>
 </sst>
 </file>
@@ -1094,10 +1145,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{631FB780-6AFF-4288-ADD9-3288FF02E2D7}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1113,7 +1164,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1172,7 +1223,7 @@
         <v>19</v>
       </c>
       <c r="H2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -1181,7 +1232,7 @@
         <v>6</v>
       </c>
       <c r="N2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -1195,48 +1246,51 @@
         <v>15</v>
       </c>
       <c r="D3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" t="s">
         <v>48</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>49</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
         <v>50</v>
       </c>
-      <c r="I3" t="s">
-        <v>51</v>
-      </c>
       <c r="K3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L3" t="s">
         <v>36</v>
       </c>
       <c r="M3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="B4">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="J4">
-        <v>2</v>
+        <v>65</v>
+      </c>
+      <c r="K4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -1250,30 +1304,27 @@
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" t="s">
-        <v>25</v>
+        <v>80</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="J5">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="N5" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>2022</v>
@@ -1282,25 +1333,25 @@
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" t="s">
-        <v>33</v>
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" t="s">
+        <v>24</v>
       </c>
       <c r="I6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L6" t="s">
-        <v>36</v>
-      </c>
-      <c r="M6" t="s">
-        <v>37</v>
+        <v>25</v>
+      </c>
+      <c r="J6">
+        <v>26</v>
+      </c>
+      <c r="N6" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -1314,48 +1365,57 @@
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F7" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I7" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="K7" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="L7" t="s">
         <v>36</v>
       </c>
       <c r="M7" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="B8">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>38</v>
+      </c>
+      <c r="F8" t="s">
+        <v>39</v>
       </c>
       <c r="I8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
+        <v>40</v>
+      </c>
+      <c r="K8" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" t="s">
+        <v>36</v>
+      </c>
+      <c r="M8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -1369,16 +1429,16 @@
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J9">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -1392,22 +1452,16 @@
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="I10" t="s">
-        <v>46</v>
-      </c>
-      <c r="J10" t="s">
-        <v>47</v>
-      </c>
-      <c r="N10" t="s">
-        <v>59</v>
+        <v>29</v>
+      </c>
+      <c r="J10">
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -1415,33 +1469,192 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>
       </c>
       <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" t="s">
+        <v>45</v>
+      </c>
+      <c r="J11" t="s">
+        <v>46</v>
+      </c>
+      <c r="N11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <v>2021</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" t="s">
+        <v>69</v>
+      </c>
+      <c r="K12" t="s">
+        <v>70</v>
+      </c>
+      <c r="L12" t="s">
+        <v>36</v>
+      </c>
+      <c r="M12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>2020</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" t="s">
         <v>53</v>
       </c>
-      <c r="E11" t="s">
+      <c r="H13" t="s">
+        <v>57</v>
+      </c>
+      <c r="I13" t="s">
         <v>54</v>
       </c>
-      <c r="H11" t="s">
-        <v>58</v>
-      </c>
-      <c r="I11" t="s">
-        <v>55</v>
-      </c>
-      <c r="J11">
+      <c r="J13">
         <v>7</v>
       </c>
-      <c r="N11" t="s">
-        <v>57</v>
+      <c r="N13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14">
+        <v>2020</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" t="s">
+        <v>73</v>
+      </c>
+      <c r="K14" t="s">
+        <v>41</v>
+      </c>
+      <c r="L14" t="s">
+        <v>36</v>
+      </c>
+      <c r="M14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15">
+        <v>2019</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" t="s">
+        <v>74</v>
+      </c>
+      <c r="K15" t="s">
+        <v>41</v>
+      </c>
+      <c r="L15" t="s">
+        <v>36</v>
+      </c>
+      <c r="M15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16">
+        <v>2018</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" t="s">
+        <v>77</v>
+      </c>
+      <c r="K16" t="s">
+        <v>79</v>
+      </c>
+      <c r="L16" t="s">
+        <v>36</v>
+      </c>
+      <c r="M16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17">
+        <v>2018</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" t="s">
+        <v>78</v>
+      </c>
+      <c r="K17" t="s">
+        <v>79</v>
+      </c>
+      <c r="L17" t="s">
+        <v>36</v>
+      </c>
+      <c r="M17" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O10">
-    <sortCondition descending="1" ref="B1:B10"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O11">
+    <sortCondition descending="1" ref="B1:B11"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update publikace + difuzni-prezkum
</commit_message>
<xml_diff>
--- a/data/publikace.xlsx
+++ b/data/publikace.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarom\Documents\GitHub\jfronc.cz\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6966FE-0408-4735-9530-D1EEA0BB5313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D57C04-7E8B-4C15-A2B2-1FB4BDEDB63E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A6FCB930-9EF3-4AF5-902E-F9B54FCB8C2A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A6FCB930-9EF3-4AF5-902E-F9B54FCB8C2A}"/>
   </bookViews>
   <sheets>
     <sheet name="publikace" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="88">
   <si>
     <t>Item Type</t>
   </si>
@@ -266,6 +266,24 @@
   </si>
   <si>
     <t>https://www.jurisprudence.cz/cz/casopis/difuzni-prezkum-okrajova-nesouladnost-a-pravni-jistota.dm-565.pdf</t>
+  </si>
+  <si>
+    <t>28-43</t>
+  </si>
+  <si>
+    <t>https://www.wintr.cz/images/sborniky/sbornik70.pdf</t>
+  </si>
+  <si>
+    <t>https://www.wintr.cz/images/sborniky/sbornik71.pdf</t>
+  </si>
+  <si>
+    <t>31-40</t>
+  </si>
+  <si>
+    <t>https://www.jurisprudence.cz/cz/casopis/usneseni-vlady-jako-pravni-predpis-terminologicky-zmatek-sui-generis.m-468.html</t>
+  </si>
+  <si>
+    <t>https://www.jurisprudence.cz/cz/casopis/usneseni-vlady-jako-pravni-predpis-terminologicky-zmatek-sui-generis.dm-468.pdf</t>
   </si>
 </sst>
 </file>
@@ -1147,8 +1165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{631FB780-6AFF-4288-ADD9-3288FF02E2D7}">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1434,11 +1452,17 @@
       <c r="E9" t="s">
         <v>17</v>
       </c>
+      <c r="H9" t="s">
+        <v>86</v>
+      </c>
       <c r="I9" t="s">
         <v>27</v>
       </c>
       <c r="J9">
         <v>1</v>
+      </c>
+      <c r="N9" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -1616,6 +1640,9 @@
       <c r="E16" t="s">
         <v>77</v>
       </c>
+      <c r="I16" t="s">
+        <v>85</v>
+      </c>
       <c r="K16" t="s">
         <v>79</v>
       </c>
@@ -1625,8 +1652,11 @@
       <c r="M16" t="s">
         <v>42</v>
       </c>
+      <c r="N16" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1642,6 +1672,9 @@
       <c r="E17" t="s">
         <v>78</v>
       </c>
+      <c r="I17" t="s">
+        <v>82</v>
+      </c>
       <c r="K17" t="s">
         <v>79</v>
       </c>
@@ -1650,6 +1683,9 @@
       </c>
       <c r="M17" t="s">
         <v>51</v>
+      </c>
+      <c r="N17" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>